<commit_message>
Cambios en el manejo de modelo de factura
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5B865-3F58-4EA5-B00F-9AFE206F4E46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A35AFF7-5201-4C9E-A7C1-1735B5C8C09E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,22 +137,22 @@
     <t>userrobot2</t>
   </si>
   <si>
-    <t>empresa</t>
-  </si>
-  <si>
     <t>descripcion</t>
   </si>
   <si>
     <t>referencia</t>
   </si>
   <si>
-    <t>referencia 1</t>
-  </si>
-  <si>
     <t>descripcion 1</t>
   </si>
   <si>
-    <t>movistar</t>
+    <t>65401</t>
+  </si>
+  <si>
+    <t>8417</t>
+  </si>
+  <si>
+    <t>convenio</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -581,13 +581,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -628,13 +628,13 @@
         <v>20</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación de question y exception a la transaccion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A35AFF7-5201-4C9E-A7C1-1735B5C8C09E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC356E-178E-4234-9B94-7154BEF2ACD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>userrobot2</t>
   </si>
   <si>
-    <t>descripcion</t>
-  </si>
-  <si>
     <t>referencia</t>
   </si>
   <si>
@@ -149,10 +146,13 @@
     <t>65401</t>
   </si>
   <si>
-    <t>8417</t>
-  </si>
-  <si>
     <t>convenio</t>
+  </si>
+  <si>
+    <t>8419</t>
+  </si>
+  <si>
+    <t>descripcionFactura</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -581,13 +581,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -628,10 +628,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
cambio de mapeo consulta detalle cuenta deposito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC356E-178E-4234-9B94-7154BEF2ACD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20130" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="3" r:id="rId1"/>
@@ -59,9 +53,21 @@
     <t>validarClave</t>
   </si>
   <si>
+    <t>convenio</t>
+  </si>
+  <si>
+    <t>descripcionFactura</t>
+  </si>
+  <si>
+    <t>referencia</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>autotest2</t>
+  </si>
+  <si>
     <t>1234</t>
   </si>
   <si>
@@ -86,6 +92,15 @@
     <t>ACTIVO</t>
   </si>
   <si>
+    <t>65401</t>
+  </si>
+  <si>
+    <t>descripcion 1</t>
+  </si>
+  <si>
+    <t>8419</t>
+  </si>
+  <si>
     <t>Orientacion</t>
   </si>
   <si>
@@ -132,34 +147,19 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>userrobot2</t>
-  </si>
-  <si>
-    <t>referencia</t>
-  </si>
-  <si>
-    <t>descripcion 1</t>
-  </si>
-  <si>
-    <t>65401</t>
-  </si>
-  <si>
-    <t>convenio</t>
-  </si>
-  <si>
-    <t>8419</t>
-  </si>
-  <si>
-    <t>descripcionFactura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,14 +183,158 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +359,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -239,12 +569,254 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -253,20 +825,64 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="Normal 2" xfId="48"/>
+    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -524,19 +1140,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
     <col min="13" max="13" width="12.125"/>
     <col min="14" max="14" width="18.375" customWidth="1"/>
@@ -581,76 +1197,78 @@
         <v>11</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>22483228</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="14.875" customWidth="1"/>
@@ -660,70 +1278,71 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactorización features y data
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/InscribirFacturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8959C36E-BE46-4163-874D-41C1DF98F557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E1C733-4EE0-4EB4-B9A6-2B74D76444F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="3" r:id="rId1"/>
@@ -146,13 +146,13 @@
     <t>Consultas</t>
   </si>
   <si>
-    <t>userrobot9</t>
-  </si>
-  <si>
-    <t>6789</t>
-  </si>
-  <si>
     <t>8418</t>
+  </si>
+  <si>
+    <t>autotest11</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
@@ -532,14 +532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="13" max="13" width="12.125"/>
-    <col min="14" max="14" width="18.375" customWidth="1"/>
+    <col min="13" max="13" width="12.08203125"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
     <col min="15" max="15" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -595,16 +595,16 @@
         <v>15</v>
       </c>
       <c r="B2" s="4">
-        <v>22493944</v>
+        <v>48646663</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>16</v>
@@ -634,7 +634,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -650,12 +650,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.58203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>